<commit_message>
updates to pintle documentation
</commit_message>
<xml_diff>
--- a/Pintle/Pintle Injector Design Documentation/Pintle_dimensions_summary.xlsx
+++ b/Pintle/Pintle Injector Design Documentation/Pintle_dimensions_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jntil\Documents\Git_Repos\liquid-engine-test-stand\Pintle\Pintle Injector Design Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFE84CC-C860-44E9-9BEA-5E4018BE22B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0803C7A4-93F0-45AD-A859-99C2D28BA60E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" xr2:uid="{4D76F15D-CEF6-45F9-953F-ACEF85900CBE}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t># of Entrances</t>
   </si>
   <si>
-    <t>Chamber diameter</t>
-  </si>
-  <si>
     <t>Flow Entrance dia.</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>Wall Thickness</t>
+  </si>
+  <si>
+    <t>Chamber radius</t>
   </si>
 </sst>
 </file>
@@ -89,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -189,23 +189,11 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -215,10 +203,22 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -538,7 +538,7 @@
   <dimension ref="C2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,284 +552,284 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
     </row>
     <row r="3" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="7" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
         <v>0.40200000000000002</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="9">
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="5">
         <v>0.40200000000000002</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.12</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="5">
         <v>0.221</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>3.125E-2</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="5">
         <v>5.9499999999999997E-2</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>12</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="5">
         <v>12</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="9">
-        <v>12</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>12</v>
+      <c r="H7" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="2">
         <f>(D14-D5)/2</f>
         <v>8.0500000000000016E-2</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="9">
+      <c r="E8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="5">
         <f>(G14-G5)/2</f>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="11">
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="7">
         <f>(D7*D6)/(PI()*D14)</f>
         <v>0.42479077337694482</v>
       </c>
-      <c r="E9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="12">
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="8">
         <f>(G7*G6)/(PI()*G14)</f>
         <v>0.53984146967987301</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>12</v>
+      <c r="H9" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="7" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.4325</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.4325</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="8" t="s">
+      <c r="D14" s="2">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="9">
-        <v>0.25</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" s="9">
-        <v>1</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.4325</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="9">
-        <v>0.4325</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="2" t="s">
+      <c r="G14" s="5">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D14" s="3">
-        <v>0.28100000000000003</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="8" t="s">
+      <c r="D15" s="2">
+        <v>0.3105</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="9">
-        <v>0.42099999999999999</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.3105</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="G15" s="5">
         <v>0.46879999999999999</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="3">
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2">
         <f>(D15-D14)/2</f>
         <v>1.4749999999999985E-2</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="9">
+      <c r="E16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="5">
         <f>(G15-G14)/2</f>
         <v>2.3900000000000005E-2</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" s="5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>